<commit_message>
Add project configuration files and update spreadsheet
Added initial JetBrains IDE project configuration files to .idea directory for Python 3.13 environment. Updated 'planilha fechamento.xlsx' with new data or formatting.
</commit_message>
<xml_diff>
--- a/planilha fechamento.xlsx
+++ b/planilha fechamento.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5115" yWindow="0" windowWidth="15375" windowHeight="7785" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -270,10 +270,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="134" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="G5" sqref="A2:G5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -463,6 +463,91 @@
       <c r="G6" t="inlineStr">
         <is>
           <t>cartão</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Noah da Mota</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Carlos Eduardo Santos</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Dr. Felipe Farias</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Luigi Barros</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Stella da Luz</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Noah da Mota</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>747.91</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>472.963.815-82</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>07/04/2024</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Carlos Eduardo Santos</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>123.2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>231.659.708-40</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>07/12/2024</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>pendente</t>
         </is>
       </c>
     </row>

</xml_diff>